<commit_message>
updating overlay and spreadsheet based on EA feedback.
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-wildfly-stig-overlay.xlsx
+++ b/cms-ars-3.1-moderate-wildfly-stig-overlay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-moderate-wildfly-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5330B4E8-6752-48CC-A592-CC389EF10C59}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BC03F9D3-A99E-514A-97D6-09CDF8A42202}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-ars-3.1-moderate-wild-stig-" sheetId="1" r:id="rId1"/>
@@ -9359,32 +9359,32 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.6484375" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.84765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.046875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="48.8984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.44921875" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="9" width="21.6484375" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="0.1484375" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6484375" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="3.34765625" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="54.046875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="32.3984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="48.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.5" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="9" width="21.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="3.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="54" style="1" customWidth="1"/>
+    <col min="14" max="14" width="32.33203125" style="1" customWidth="1"/>
     <col min="15" max="15" width="17.5" style="1" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="15" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="19.34765625" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="13.69921875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="18.84765625" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="21.6484375" style="1"/>
+    <col min="17" max="17" width="19.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="18.83203125" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="21.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="24" customHeight="1">
@@ -9446,7 +9446,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="409.5">
+    <row r="2" spans="1:19" ht="409.6">
       <c r="A2" s="3" t="s">
         <v>274</v>
       </c>
@@ -9501,7 +9501,7 @@
       </c>
       <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:19" ht="409.5">
+    <row r="3" spans="1:19" ht="409.6">
       <c r="A3" s="5" t="s">
         <v>131</v>
       </c>
@@ -9556,7 +9556,7 @@
       </c>
       <c r="S3" s="2"/>
     </row>
-    <row r="4" spans="1:19" ht="409.5">
+    <row r="4" spans="1:19" ht="409.6">
       <c r="A4" s="3" t="s">
         <v>564</v>
       </c>
@@ -9611,7 +9611,7 @@
       </c>
       <c r="S4" s="2"/>
     </row>
-    <row r="5" spans="1:19" ht="409.5">
+    <row r="5" spans="1:19" ht="409.6">
       <c r="A5" s="3" t="s">
         <v>430</v>
       </c>
@@ -9666,7 +9666,7 @@
       </c>
       <c r="S5" s="2"/>
     </row>
-    <row r="6" spans="1:19" ht="409.5">
+    <row r="6" spans="1:19" ht="409.6">
       <c r="A6" s="3" t="s">
         <v>143</v>
       </c>
@@ -9721,7 +9721,7 @@
       </c>
       <c r="S6" s="2"/>
     </row>
-    <row r="7" spans="1:19" ht="409.5">
+    <row r="7" spans="1:19" ht="409.6">
       <c r="A7" s="3" t="s">
         <v>586</v>
       </c>
@@ -9776,7 +9776,7 @@
       </c>
       <c r="S7" s="2"/>
     </row>
-    <row r="8" spans="1:19" ht="409.5">
+    <row r="8" spans="1:19" ht="409.6">
       <c r="A8" s="3" t="s">
         <v>64</v>
       </c>
@@ -9831,7 +9831,7 @@
       </c>
       <c r="S8" s="2"/>
     </row>
-    <row r="9" spans="1:19" ht="409.5">
+    <row r="9" spans="1:19" ht="409.6">
       <c r="A9" s="3" t="s">
         <v>641</v>
       </c>
@@ -9886,7 +9886,7 @@
       </c>
       <c r="S9" s="2"/>
     </row>
-    <row r="10" spans="1:19" ht="409.5">
+    <row r="10" spans="1:19" ht="409.6">
       <c r="A10" s="3" t="s">
         <v>420</v>
       </c>
@@ -9941,7 +9941,7 @@
       </c>
       <c r="S10" s="7"/>
     </row>
-    <row r="11" spans="1:19" ht="409.5">
+    <row r="11" spans="1:19" ht="409.6">
       <c r="A11" s="3" t="s">
         <v>105</v>
       </c>
@@ -9996,7 +9996,7 @@
       </c>
       <c r="S11" s="2"/>
     </row>
-    <row r="12" spans="1:19" ht="409.5">
+    <row r="12" spans="1:19" ht="409.6">
       <c r="A12" s="3" t="s">
         <v>539</v>
       </c>
@@ -10051,7 +10051,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:19" ht="409.5">
+    <row r="13" spans="1:19" ht="409.6">
       <c r="A13" s="5" t="s">
         <v>50</v>
       </c>
@@ -10108,7 +10108,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="409.5">
+    <row r="14" spans="1:19" ht="409.6">
       <c r="A14" s="3" t="s">
         <v>605</v>
       </c>
@@ -10163,7 +10163,7 @@
       </c>
       <c r="S14" s="2"/>
     </row>
-    <row r="15" spans="1:19" ht="409.5">
+    <row r="15" spans="1:19" ht="409.6">
       <c r="A15" s="3" t="s">
         <v>411</v>
       </c>
@@ -10218,7 +10218,7 @@
       </c>
       <c r="S15" s="2"/>
     </row>
-    <row r="16" spans="1:19" ht="409.5">
+    <row r="16" spans="1:19" ht="409.6">
       <c r="A16" s="3" t="s">
         <v>360</v>
       </c>
@@ -10273,7 +10273,7 @@
       </c>
       <c r="S16" s="2"/>
     </row>
-    <row r="17" spans="1:19" ht="409.5">
+    <row r="17" spans="1:19" ht="409.6">
       <c r="A17" s="3" t="s">
         <v>719</v>
       </c>
@@ -10328,7 +10328,7 @@
       </c>
       <c r="S17" s="2"/>
     </row>
-    <row r="18" spans="1:19" ht="409.5">
+    <row r="18" spans="1:19" ht="409.6">
       <c r="A18" s="3" t="s">
         <v>225</v>
       </c>
@@ -10383,7 +10383,7 @@
       </c>
       <c r="S18" s="2"/>
     </row>
-    <row r="19" spans="1:19" ht="409.5">
+    <row r="19" spans="1:19" ht="409.6">
       <c r="A19" s="3" t="s">
         <v>794</v>
       </c>
@@ -10438,7 +10438,7 @@
       </c>
       <c r="S19" s="2"/>
     </row>
-    <row r="20" spans="1:19" ht="409.5">
+    <row r="20" spans="1:19" ht="409.6">
       <c r="A20" s="3" t="s">
         <v>469</v>
       </c>
@@ -10493,7 +10493,7 @@
       </c>
       <c r="S20" s="2"/>
     </row>
-    <row r="21" spans="1:19" ht="409.5">
+    <row r="21" spans="1:19" ht="409.6">
       <c r="A21" s="3" t="s">
         <v>300</v>
       </c>
@@ -10548,7 +10548,7 @@
       </c>
       <c r="S21" s="2"/>
     </row>
-    <row r="22" spans="1:19" ht="409.5">
+    <row r="22" spans="1:19" ht="409.6">
       <c r="A22" s="3" t="s">
         <v>661</v>
       </c>
@@ -10603,7 +10603,7 @@
       </c>
       <c r="S22" s="2"/>
     </row>
-    <row r="23" spans="1:19" ht="409.5">
+    <row r="23" spans="1:19" ht="409.6">
       <c r="A23" s="3" t="s">
         <v>211</v>
       </c>
@@ -10658,7 +10658,7 @@
       </c>
       <c r="S23" s="2"/>
     </row>
-    <row r="24" spans="1:19" ht="409.5">
+    <row r="24" spans="1:19" ht="409.6">
       <c r="A24" s="3" t="s">
         <v>780</v>
       </c>
@@ -10713,7 +10713,7 @@
       </c>
       <c r="S24" s="2"/>
     </row>
-    <row r="25" spans="1:19" ht="409.5">
+    <row r="25" spans="1:19" ht="409.6">
       <c r="A25" s="5" t="s">
         <v>456</v>
       </c>
@@ -10768,7 +10768,7 @@
       </c>
       <c r="S25" s="7"/>
     </row>
-    <row r="26" spans="1:19" ht="409.5">
+    <row r="26" spans="1:19" ht="409.6">
       <c r="A26" s="3" t="s">
         <v>169</v>
       </c>
@@ -10823,7 +10823,7 @@
       </c>
       <c r="S26" s="2"/>
     </row>
-    <row r="27" spans="1:19" ht="409.5">
+    <row r="27" spans="1:19" ht="409.6">
       <c r="A27" s="3" t="s">
         <v>745</v>
       </c>
@@ -10878,7 +10878,7 @@
       </c>
       <c r="S27" s="2"/>
     </row>
-    <row r="28" spans="1:19" ht="409.5">
+    <row r="28" spans="1:19" ht="409.6">
       <c r="A28" s="3" t="s">
         <v>312</v>
       </c>
@@ -10933,7 +10933,7 @@
       </c>
       <c r="S28" s="2"/>
     </row>
-    <row r="29" spans="1:19" ht="409.5">
+    <row r="29" spans="1:19" ht="409.6">
       <c r="A29" s="3" t="s">
         <v>673</v>
       </c>
@@ -10988,7 +10988,7 @@
       </c>
       <c r="S29" s="2"/>
     </row>
-    <row r="30" spans="1:19" ht="409.5">
+    <row r="30" spans="1:19" ht="409.6">
       <c r="A30" s="3" t="s">
         <v>493</v>
       </c>
@@ -11043,7 +11043,7 @@
       </c>
       <c r="S30" s="2"/>
     </row>
-    <row r="31" spans="1:19" ht="409.5">
+    <row r="31" spans="1:19" ht="409.6">
       <c r="A31" s="3" t="s">
         <v>262</v>
       </c>
@@ -11098,7 +11098,7 @@
       </c>
       <c r="S31" s="2"/>
     </row>
-    <row r="32" spans="1:19" ht="409.5">
+    <row r="32" spans="1:19" ht="409.6">
       <c r="A32" s="3" t="s">
         <v>830</v>
       </c>
@@ -11153,7 +11153,7 @@
       </c>
       <c r="S32" s="2"/>
     </row>
-    <row r="33" spans="1:19" ht="409.5">
+    <row r="33" spans="1:19" ht="409.6">
       <c r="A33" s="5" t="s">
         <v>346</v>
       </c>
@@ -11208,7 +11208,7 @@
       </c>
       <c r="S33" s="2"/>
     </row>
-    <row r="34" spans="1:19" ht="409.5">
+    <row r="34" spans="1:19" ht="409.6">
       <c r="A34" s="3" t="s">
         <v>705</v>
       </c>
@@ -11263,7 +11263,7 @@
       </c>
       <c r="S34" s="2"/>
     </row>
-    <row r="35" spans="1:19" ht="409.5">
+    <row r="35" spans="1:19" ht="409.6">
       <c r="A35" s="5" t="s">
         <v>526</v>
       </c>
@@ -11318,7 +11318,7 @@
       </c>
       <c r="S35" s="2"/>
     </row>
-    <row r="36" spans="1:19" ht="409.5">
+    <row r="36" spans="1:19" ht="409.6">
       <c r="A36" s="5" t="s">
         <v>576</v>
       </c>
@@ -11373,7 +11373,7 @@
       </c>
       <c r="S36" s="2"/>
     </row>
-    <row r="37" spans="1:19" ht="409.5">
+    <row r="37" spans="1:19" ht="409.6">
       <c r="A37" s="3" t="s">
         <v>155</v>
       </c>
@@ -11428,7 +11428,7 @@
       </c>
       <c r="S37" s="2"/>
     </row>
-    <row r="38" spans="1:19" ht="409.5">
+    <row r="38" spans="1:19" ht="409.6">
       <c r="A38" s="5" t="s">
         <v>628</v>
       </c>
@@ -11483,7 +11483,7 @@
       </c>
       <c r="S38" s="2"/>
     </row>
-    <row r="39" spans="1:19" ht="409.5">
+    <row r="39" spans="1:19" ht="409.6">
       <c r="A39" s="3" t="s">
         <v>78</v>
       </c>
@@ -11538,7 +11538,7 @@
       </c>
       <c r="S39" s="2"/>
     </row>
-    <row r="40" spans="1:19" ht="409.5">
+    <row r="40" spans="1:19" ht="409.6">
       <c r="A40" s="3" t="s">
         <v>399</v>
       </c>
@@ -11593,7 +11593,7 @@
       </c>
       <c r="S40" s="2"/>
     </row>
-    <row r="41" spans="1:19" ht="409.5">
+    <row r="41" spans="1:19" ht="409.6">
       <c r="A41" s="3" t="s">
         <v>553</v>
       </c>
@@ -11648,7 +11648,7 @@
       </c>
       <c r="S41" s="2"/>
     </row>
-    <row r="42" spans="1:19" ht="409.5">
+    <row r="42" spans="1:19" ht="409.6">
       <c r="A42" s="3" t="s">
         <v>92</v>
       </c>
@@ -11703,7 +11703,7 @@
       </c>
       <c r="S42" s="2"/>
     </row>
-    <row r="43" spans="1:19" ht="409.5">
+    <row r="43" spans="1:19" ht="409.6">
       <c r="A43" s="3" t="s">
         <v>616</v>
       </c>
@@ -11758,7 +11758,7 @@
       </c>
       <c r="S43" s="2"/>
     </row>
-    <row r="44" spans="1:19" ht="409.5">
+    <row r="44" spans="1:19" ht="409.6">
       <c r="A44" s="3" t="s">
         <v>36</v>
       </c>
@@ -11813,7 +11813,7 @@
       </c>
       <c r="S44" s="2"/>
     </row>
-    <row r="45" spans="1:19" ht="409.5">
+    <row r="45" spans="1:19" ht="409.6">
       <c r="A45" s="3" t="s">
         <v>386</v>
       </c>
@@ -11868,7 +11868,7 @@
       </c>
       <c r="S45" s="2"/>
     </row>
-    <row r="46" spans="1:19" ht="409.5">
+    <row r="46" spans="1:19" ht="409.6">
       <c r="A46" s="3" t="s">
         <v>372</v>
       </c>
@@ -11923,7 +11923,7 @@
       </c>
       <c r="S46" s="2"/>
     </row>
-    <row r="47" spans="1:19" ht="409.5">
+    <row r="47" spans="1:19" ht="409.6">
       <c r="A47" s="3" t="s">
         <v>732</v>
       </c>
@@ -11978,7 +11978,7 @@
       </c>
       <c r="S47" s="2"/>
     </row>
-    <row r="48" spans="1:19" ht="409.5">
+    <row r="48" spans="1:19" ht="409.6">
       <c r="A48" s="3" t="s">
         <v>238</v>
       </c>
@@ -12033,7 +12033,7 @@
       </c>
       <c r="S48" s="2"/>
     </row>
-    <row r="49" spans="1:19" ht="409.5">
+    <row r="49" spans="1:19" ht="409.6">
       <c r="A49" s="3" t="s">
         <v>806</v>
       </c>
@@ -12088,7 +12088,7 @@
       </c>
       <c r="S49" s="2"/>
     </row>
-    <row r="50" spans="1:19" ht="409.5">
+    <row r="50" spans="1:19" ht="409.6">
       <c r="A50" s="5" t="s">
         <v>482</v>
       </c>
@@ -12143,7 +12143,7 @@
       </c>
       <c r="S50" s="2"/>
     </row>
-    <row r="51" spans="1:19" ht="409.5">
+    <row r="51" spans="1:19" ht="409.6">
       <c r="A51" s="3" t="s">
         <v>287</v>
       </c>
@@ -12198,7 +12198,7 @@
       </c>
       <c r="S51" s="2"/>
     </row>
-    <row r="52" spans="1:19" ht="409.5">
+    <row r="52" spans="1:19" ht="409.6">
       <c r="A52" s="3" t="s">
         <v>650</v>
       </c>
@@ -12253,7 +12253,7 @@
       </c>
       <c r="S52" s="2"/>
     </row>
-    <row r="53" spans="1:19" ht="409.5">
+    <row r="53" spans="1:19" ht="409.6">
       <c r="A53" s="3" t="s">
         <v>197</v>
       </c>
@@ -12308,7 +12308,7 @@
       </c>
       <c r="S53" s="2"/>
     </row>
-    <row r="54" spans="1:19" ht="409.5">
+    <row r="54" spans="1:19" ht="409.6">
       <c r="A54" s="5" t="s">
         <v>769</v>
       </c>
@@ -12363,7 +12363,7 @@
       </c>
       <c r="S54" s="2"/>
     </row>
-    <row r="55" spans="1:19" ht="409.5">
+    <row r="55" spans="1:19" ht="409.6">
       <c r="A55" s="3" t="s">
         <v>442</v>
       </c>
@@ -12418,7 +12418,7 @@
       </c>
       <c r="S55" s="2"/>
     </row>
-    <row r="56" spans="1:19" ht="409.5">
+    <row r="56" spans="1:19" ht="409.6">
       <c r="A56" s="3" t="s">
         <v>183</v>
       </c>
@@ -12473,7 +12473,7 @@
       </c>
       <c r="S56" s="2"/>
     </row>
-    <row r="57" spans="1:19" ht="409.5">
+    <row r="57" spans="1:19" ht="409.6">
       <c r="A57" s="3" t="s">
         <v>757</v>
       </c>
@@ -12528,7 +12528,7 @@
       </c>
       <c r="S57" s="2"/>
     </row>
-    <row r="58" spans="1:19" ht="409.5">
+    <row r="58" spans="1:19" ht="409.6">
       <c r="A58" s="3" t="s">
         <v>323</v>
       </c>
@@ -12583,7 +12583,7 @@
       </c>
       <c r="S58" s="2"/>
     </row>
-    <row r="59" spans="1:19" ht="409.5">
+    <row r="59" spans="1:19" ht="409.6">
       <c r="A59" s="3" t="s">
         <v>684</v>
       </c>
@@ -12638,7 +12638,7 @@
       </c>
       <c r="S59" s="2"/>
     </row>
-    <row r="60" spans="1:19" ht="409.5">
+    <row r="60" spans="1:19" ht="409.6">
       <c r="A60" s="3" t="s">
         <v>505</v>
       </c>
@@ -12693,7 +12693,7 @@
       </c>
       <c r="S60" s="2"/>
     </row>
-    <row r="61" spans="1:19" ht="409.5">
+    <row r="61" spans="1:19" ht="409.6">
       <c r="A61" s="3" t="s">
         <v>252</v>
       </c>
@@ -12748,7 +12748,7 @@
       </c>
       <c r="S61" s="2"/>
     </row>
-    <row r="62" spans="1:19" ht="409.5">
+    <row r="62" spans="1:19" ht="409.6">
       <c r="A62" s="3" t="s">
         <v>820</v>
       </c>
@@ -12803,7 +12803,7 @@
       </c>
       <c r="S62" s="2"/>
     </row>
-    <row r="63" spans="1:19" ht="409.5">
+    <row r="63" spans="1:19" ht="409.6">
       <c r="A63" s="3" t="s">
         <v>337</v>
       </c>
@@ -12858,7 +12858,7 @@
       </c>
       <c r="S63" s="2"/>
     </row>
-    <row r="64" spans="1:19" ht="409.5">
+    <row r="64" spans="1:19" ht="409.6">
       <c r="A64" s="3" t="s">
         <v>696</v>
       </c>
@@ -12913,7 +12913,7 @@
       </c>
       <c r="S64" s="2"/>
     </row>
-    <row r="65" spans="1:19" ht="409.5">
+    <row r="65" spans="1:19" ht="409.6">
       <c r="A65" s="3" t="s">
         <v>516</v>
       </c>
@@ -12968,7 +12968,7 @@
       </c>
       <c r="S65" s="2"/>
     </row>
-    <row r="66" spans="1:19" ht="326.05" customHeight="1">
+    <row r="66" spans="1:19" ht="326" customHeight="1">
       <c r="A66" s="3" t="s">
         <v>22</v>
       </c>
@@ -13023,7 +13023,7 @@
       </c>
       <c r="S66" s="2"/>
     </row>
-    <row r="67" spans="1:19" ht="409.5">
+    <row r="67" spans="1:19" ht="409.6">
       <c r="A67" s="5" t="s">
         <v>596</v>
       </c>
@@ -13078,7 +13078,7 @@
       </c>
       <c r="S67" s="2"/>
     </row>
-    <row r="68" spans="1:19" ht="409.5">
+    <row r="68" spans="1:19" ht="409.6">
       <c r="A68" s="5" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
Adjustments to be consistent with Lifecycle SOP
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-wildfly-stig-overlay.xlsx
+++ b/cms-ars-3.1-moderate-wildfly-stig-overlay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-moderate-wildfly-stig-overlay/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BC03F9D3-A99E-514A-97D6-09CDF8A42202}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B12ED36-D865-4F69-A27C-5963D5C89C04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-ars-3.1-moderate-wild-stig-" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1092" uniqueCount="862">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1096" uniqueCount="862">
   <si>
     <t>title</t>
   </si>
@@ -8188,90 +8188,6 @@
 desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since the related security control is not included in CMS ARS 3.1'</t>
   </si>
   <si>
-    <r>
-      <t>["AU-4</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (1)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", "Rev_4"]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>["CM-5</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (6)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", "Rev_4"]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>["SC-23</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (5)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>", "Rev_4"]</t>
-    </r>
-  </si>
-  <si>
     <t>The Wildfly product is available as Open Source; however, the Red Hat
   vendor provides updates, patches and support for the JBoss product.  It is
   imperative that patches and updates be applied to Wildfly in a timely manner as
@@ -8440,12 +8356,21 @@
   policy.</t>
     </r>
   </si>
+  <si>
+    <t>["CM-5 (6)", "Rev_4"]</t>
+  </si>
+  <si>
+    <t>["AU-4 (1)", "Rev_4"]</t>
+  </si>
+  <si>
+    <t>["SC-23 (5)", "Rev_4"]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -8612,6 +8537,12 @@
       <strike/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -8979,7 +8910,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -9000,6 +8931,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9047,7 +8981,16 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -9359,32 +9302,32 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72"/>
+      <selection pane="bottomRight" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="21.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="21.6484375" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.84765625" style="1" customWidth="1"/>
     <col min="3" max="3" width="25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="48.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="48.84765625" style="1" customWidth="1"/>
     <col min="5" max="5" width="38.5" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="9" width="21.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="0.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="3.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="9" width="21.6484375" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0.1484375" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6484375" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="3.34765625" style="1" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="54" style="1" customWidth="1"/>
-    <col min="14" max="14" width="32.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="32.34765625" style="1" customWidth="1"/>
     <col min="15" max="15" width="17.5" style="1" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="15" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="19.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="13.6640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="18.83203125" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="21.6640625" style="1"/>
+    <col min="17" max="17" width="19.34765625" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6484375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="18.84765625" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="21.6484375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="24" customHeight="1">
@@ -9401,7 +9344,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -9446,7 +9389,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="409.6">
+    <row r="2" spans="1:19" ht="409.5">
       <c r="A2" s="3" t="s">
         <v>274</v>
       </c>
@@ -9501,7 +9444,7 @@
       </c>
       <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:19" ht="409.6">
+    <row r="3" spans="1:19" ht="409.5">
       <c r="A3" s="5" t="s">
         <v>131</v>
       </c>
@@ -9556,7 +9499,7 @@
       </c>
       <c r="S3" s="2"/>
     </row>
-    <row r="4" spans="1:19" ht="409.6">
+    <row r="4" spans="1:19" ht="409.5">
       <c r="A4" s="3" t="s">
         <v>564</v>
       </c>
@@ -9611,7 +9554,7 @@
       </c>
       <c r="S4" s="2"/>
     </row>
-    <row r="5" spans="1:19" ht="409.6">
+    <row r="5" spans="1:19" ht="409.5">
       <c r="A5" s="3" t="s">
         <v>430</v>
       </c>
@@ -9622,7 +9565,7 @@
         <v>428</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>429</v>
@@ -9666,7 +9609,7 @@
       </c>
       <c r="S5" s="2"/>
     </row>
-    <row r="6" spans="1:19" ht="409.6">
+    <row r="6" spans="1:19" ht="409.5">
       <c r="A6" s="3" t="s">
         <v>143</v>
       </c>
@@ -9721,7 +9664,7 @@
       </c>
       <c r="S6" s="2"/>
     </row>
-    <row r="7" spans="1:19" ht="409.6">
+    <row r="7" spans="1:19" ht="409.5">
       <c r="A7" s="3" t="s">
         <v>586</v>
       </c>
@@ -9776,7 +9719,7 @@
       </c>
       <c r="S7" s="2"/>
     </row>
-    <row r="8" spans="1:19" ht="409.6">
+    <row r="8" spans="1:19" ht="409.5">
       <c r="A8" s="3" t="s">
         <v>64</v>
       </c>
@@ -9831,7 +9774,7 @@
       </c>
       <c r="S8" s="2"/>
     </row>
-    <row r="9" spans="1:19" ht="409.6">
+    <row r="9" spans="1:19" ht="409.5">
       <c r="A9" s="3" t="s">
         <v>641</v>
       </c>
@@ -9886,7 +9829,7 @@
       </c>
       <c r="S9" s="2"/>
     </row>
-    <row r="10" spans="1:19" ht="409.6">
+    <row r="10" spans="1:19" ht="409.5">
       <c r="A10" s="3" t="s">
         <v>420</v>
       </c>
@@ -9897,7 +9840,7 @@
         <v>418</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>419</v>
@@ -9941,7 +9884,7 @@
       </c>
       <c r="S10" s="7"/>
     </row>
-    <row r="11" spans="1:19" ht="409.6">
+    <row r="11" spans="1:19" ht="409.5">
       <c r="A11" s="3" t="s">
         <v>105</v>
       </c>
@@ -9996,7 +9939,7 @@
       </c>
       <c r="S11" s="2"/>
     </row>
-    <row r="12" spans="1:19" ht="409.6">
+    <row r="12" spans="1:19" ht="409.5">
       <c r="A12" s="3" t="s">
         <v>539</v>
       </c>
@@ -10051,7 +9994,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:19" ht="409.6">
+    <row r="13" spans="1:19" ht="409.5">
       <c r="A13" s="5" t="s">
         <v>50</v>
       </c>
@@ -10108,7 +10051,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="409.6">
+    <row r="14" spans="1:19" ht="409.5">
       <c r="A14" s="3" t="s">
         <v>605</v>
       </c>
@@ -10163,7 +10106,7 @@
       </c>
       <c r="S14" s="2"/>
     </row>
-    <row r="15" spans="1:19" ht="409.6">
+    <row r="15" spans="1:19" ht="409.5">
       <c r="A15" s="3" t="s">
         <v>411</v>
       </c>
@@ -10218,7 +10161,7 @@
       </c>
       <c r="S15" s="2"/>
     </row>
-    <row r="16" spans="1:19" ht="409.6">
+    <row r="16" spans="1:19" ht="409.5">
       <c r="A16" s="3" t="s">
         <v>360</v>
       </c>
@@ -10273,7 +10216,7 @@
       </c>
       <c r="S16" s="2"/>
     </row>
-    <row r="17" spans="1:19" ht="409.6">
+    <row r="17" spans="1:19" ht="409.5">
       <c r="A17" s="3" t="s">
         <v>719</v>
       </c>
@@ -10328,7 +10271,7 @@
       </c>
       <c r="S17" s="2"/>
     </row>
-    <row r="18" spans="1:19" ht="409.6">
+    <row r="18" spans="1:19" ht="409.5">
       <c r="A18" s="3" t="s">
         <v>225</v>
       </c>
@@ -10383,7 +10326,7 @@
       </c>
       <c r="S18" s="2"/>
     </row>
-    <row r="19" spans="1:19" ht="409.6">
+    <row r="19" spans="1:19" ht="409.5">
       <c r="A19" s="3" t="s">
         <v>794</v>
       </c>
@@ -10438,7 +10381,7 @@
       </c>
       <c r="S19" s="2"/>
     </row>
-    <row r="20" spans="1:19" ht="409.6">
+    <row r="20" spans="1:19" ht="409.5">
       <c r="A20" s="3" t="s">
         <v>469</v>
       </c>
@@ -10493,7 +10436,7 @@
       </c>
       <c r="S20" s="2"/>
     </row>
-    <row r="21" spans="1:19" ht="409.6">
+    <row r="21" spans="1:19" ht="409.5">
       <c r="A21" s="3" t="s">
         <v>300</v>
       </c>
@@ -10548,7 +10491,7 @@
       </c>
       <c r="S21" s="2"/>
     </row>
-    <row r="22" spans="1:19" ht="409.6">
+    <row r="22" spans="1:19" ht="409.5">
       <c r="A22" s="3" t="s">
         <v>661</v>
       </c>
@@ -10603,7 +10546,7 @@
       </c>
       <c r="S22" s="2"/>
     </row>
-    <row r="23" spans="1:19" ht="409.6">
+    <row r="23" spans="1:19" ht="409.5">
       <c r="A23" s="3" t="s">
         <v>211</v>
       </c>
@@ -10658,7 +10601,7 @@
       </c>
       <c r="S23" s="2"/>
     </row>
-    <row r="24" spans="1:19" ht="409.6">
+    <row r="24" spans="1:19" ht="409.5">
       <c r="A24" s="3" t="s">
         <v>780</v>
       </c>
@@ -10713,12 +10656,12 @@
       </c>
       <c r="S24" s="2"/>
     </row>
-    <row r="25" spans="1:19" ht="409.6">
+    <row r="25" spans="1:19" ht="409.5">
       <c r="A25" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="B25" s="2">
-        <v>0.5</v>
+      <c r="B25" s="6">
+        <v>0</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>452</v>
@@ -10763,12 +10706,14 @@
       <c r="Q25" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="R25" s="6" t="s">
-        <v>853</v>
-      </c>
-      <c r="S25" s="7"/>
+      <c r="R25" s="8" t="s">
+        <v>859</v>
+      </c>
+      <c r="S25" s="6" t="s">
+        <v>851</v>
+      </c>
     </row>
-    <row r="26" spans="1:19" ht="409.6">
+    <row r="26" spans="1:19" ht="409.5">
       <c r="A26" s="3" t="s">
         <v>169</v>
       </c>
@@ -10823,7 +10768,7 @@
       </c>
       <c r="S26" s="2"/>
     </row>
-    <row r="27" spans="1:19" ht="409.6">
+    <row r="27" spans="1:19" ht="409.5">
       <c r="A27" s="3" t="s">
         <v>745</v>
       </c>
@@ -10878,7 +10823,7 @@
       </c>
       <c r="S27" s="2"/>
     </row>
-    <row r="28" spans="1:19" ht="409.6">
+    <row r="28" spans="1:19" ht="409.5">
       <c r="A28" s="3" t="s">
         <v>312</v>
       </c>
@@ -10933,7 +10878,7 @@
       </c>
       <c r="S28" s="2"/>
     </row>
-    <row r="29" spans="1:19" ht="409.6">
+    <row r="29" spans="1:19" ht="409.5">
       <c r="A29" s="3" t="s">
         <v>673</v>
       </c>
@@ -10988,7 +10933,7 @@
       </c>
       <c r="S29" s="2"/>
     </row>
-    <row r="30" spans="1:19" ht="409.6">
+    <row r="30" spans="1:19" ht="409.5">
       <c r="A30" s="3" t="s">
         <v>493</v>
       </c>
@@ -11043,7 +10988,7 @@
       </c>
       <c r="S30" s="2"/>
     </row>
-    <row r="31" spans="1:19" ht="409.6">
+    <row r="31" spans="1:19" ht="409.5">
       <c r="A31" s="3" t="s">
         <v>262</v>
       </c>
@@ -11098,7 +11043,7 @@
       </c>
       <c r="S31" s="2"/>
     </row>
-    <row r="32" spans="1:19" ht="409.6">
+    <row r="32" spans="1:19" ht="409.5">
       <c r="A32" s="3" t="s">
         <v>830</v>
       </c>
@@ -11153,7 +11098,7 @@
       </c>
       <c r="S32" s="2"/>
     </row>
-    <row r="33" spans="1:19" ht="409.6">
+    <row r="33" spans="1:19" ht="409.5">
       <c r="A33" s="5" t="s">
         <v>346</v>
       </c>
@@ -11208,7 +11153,7 @@
       </c>
       <c r="S33" s="2"/>
     </row>
-    <row r="34" spans="1:19" ht="409.6">
+    <row r="34" spans="1:19" ht="409.5">
       <c r="A34" s="3" t="s">
         <v>705</v>
       </c>
@@ -11219,7 +11164,7 @@
         <v>702</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>703</v>
@@ -11263,7 +11208,7 @@
       </c>
       <c r="S34" s="2"/>
     </row>
-    <row r="35" spans="1:19" ht="409.6">
+    <row r="35" spans="1:19" ht="409.5">
       <c r="A35" s="5" t="s">
         <v>526</v>
       </c>
@@ -11274,7 +11219,7 @@
         <v>523</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>524</v>
@@ -11318,7 +11263,7 @@
       </c>
       <c r="S35" s="2"/>
     </row>
-    <row r="36" spans="1:19" ht="409.6">
+    <row r="36" spans="1:19" ht="409.5">
       <c r="A36" s="5" t="s">
         <v>576</v>
       </c>
@@ -11373,7 +11318,7 @@
       </c>
       <c r="S36" s="2"/>
     </row>
-    <row r="37" spans="1:19" ht="409.6">
+    <row r="37" spans="1:19" ht="409.5">
       <c r="A37" s="3" t="s">
         <v>155</v>
       </c>
@@ -11428,7 +11373,7 @@
       </c>
       <c r="S37" s="2"/>
     </row>
-    <row r="38" spans="1:19" ht="409.6">
+    <row r="38" spans="1:19" ht="409.5">
       <c r="A38" s="5" t="s">
         <v>628</v>
       </c>
@@ -11439,7 +11384,7 @@
         <v>845</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>626</v>
@@ -11483,7 +11428,7 @@
       </c>
       <c r="S38" s="2"/>
     </row>
-    <row r="39" spans="1:19" ht="409.6">
+    <row r="39" spans="1:19" ht="409.5">
       <c r="A39" s="3" t="s">
         <v>78</v>
       </c>
@@ -11538,7 +11483,7 @@
       </c>
       <c r="S39" s="2"/>
     </row>
-    <row r="40" spans="1:19" ht="409.6">
+    <row r="40" spans="1:19" ht="409.5">
       <c r="A40" s="3" t="s">
         <v>399</v>
       </c>
@@ -11593,7 +11538,7 @@
       </c>
       <c r="S40" s="2"/>
     </row>
-    <row r="41" spans="1:19" ht="409.6">
+    <row r="41" spans="1:19" ht="409.5">
       <c r="A41" s="3" t="s">
         <v>553</v>
       </c>
@@ -11648,7 +11593,7 @@
       </c>
       <c r="S41" s="2"/>
     </row>
-    <row r="42" spans="1:19" ht="409.6">
+    <row r="42" spans="1:19" ht="409.5">
       <c r="A42" s="3" t="s">
         <v>92</v>
       </c>
@@ -11703,7 +11648,7 @@
       </c>
       <c r="S42" s="2"/>
     </row>
-    <row r="43" spans="1:19" ht="409.6">
+    <row r="43" spans="1:19" ht="409.5">
       <c r="A43" s="3" t="s">
         <v>616</v>
       </c>
@@ -11758,7 +11703,7 @@
       </c>
       <c r="S43" s="2"/>
     </row>
-    <row r="44" spans="1:19" ht="409.6">
+    <row r="44" spans="1:19" ht="409.5">
       <c r="A44" s="3" t="s">
         <v>36</v>
       </c>
@@ -11813,7 +11758,7 @@
       </c>
       <c r="S44" s="2"/>
     </row>
-    <row r="45" spans="1:19" ht="409.6">
+    <row r="45" spans="1:19" ht="409.5">
       <c r="A45" s="3" t="s">
         <v>386</v>
       </c>
@@ -11868,7 +11813,7 @@
       </c>
       <c r="S45" s="2"/>
     </row>
-    <row r="46" spans="1:19" ht="409.6">
+    <row r="46" spans="1:19" ht="409.5">
       <c r="A46" s="3" t="s">
         <v>372</v>
       </c>
@@ -11923,7 +11868,7 @@
       </c>
       <c r="S46" s="2"/>
     </row>
-    <row r="47" spans="1:19" ht="409.6">
+    <row r="47" spans="1:19" ht="409.5">
       <c r="A47" s="3" t="s">
         <v>732</v>
       </c>
@@ -11978,7 +11923,7 @@
       </c>
       <c r="S47" s="2"/>
     </row>
-    <row r="48" spans="1:19" ht="409.6">
+    <row r="48" spans="1:19" ht="409.5">
       <c r="A48" s="3" t="s">
         <v>238</v>
       </c>
@@ -12033,7 +11978,7 @@
       </c>
       <c r="S48" s="2"/>
     </row>
-    <row r="49" spans="1:19" ht="409.6">
+    <row r="49" spans="1:19" ht="409.5">
       <c r="A49" s="3" t="s">
         <v>806</v>
       </c>
@@ -12088,12 +12033,12 @@
       </c>
       <c r="S49" s="2"/>
     </row>
-    <row r="50" spans="1:19" ht="409.6">
+    <row r="50" spans="1:19" ht="409.5">
       <c r="A50" s="5" t="s">
         <v>482</v>
       </c>
-      <c r="B50" s="2">
-        <v>0.5</v>
+      <c r="B50" s="6">
+        <v>0</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>478</v>
@@ -12138,12 +12083,14 @@
       <c r="Q50" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="R50" s="6" t="s">
-        <v>852</v>
-      </c>
-      <c r="S50" s="2"/>
+      <c r="R50" s="8" t="s">
+        <v>860</v>
+      </c>
+      <c r="S50" s="6" t="s">
+        <v>851</v>
+      </c>
     </row>
-    <row r="51" spans="1:19" ht="409.6">
+    <row r="51" spans="1:19" ht="409.5">
       <c r="A51" s="3" t="s">
         <v>287</v>
       </c>
@@ -12198,7 +12145,7 @@
       </c>
       <c r="S51" s="2"/>
     </row>
-    <row r="52" spans="1:19" ht="409.6">
+    <row r="52" spans="1:19" ht="409.5">
       <c r="A52" s="3" t="s">
         <v>650</v>
       </c>
@@ -12253,7 +12200,7 @@
       </c>
       <c r="S52" s="2"/>
     </row>
-    <row r="53" spans="1:19" ht="409.6">
+    <row r="53" spans="1:19" ht="409.5">
       <c r="A53" s="3" t="s">
         <v>197</v>
       </c>
@@ -12308,12 +12255,12 @@
       </c>
       <c r="S53" s="2"/>
     </row>
-    <row r="54" spans="1:19" ht="409.6">
+    <row r="54" spans="1:19" ht="409.5">
       <c r="A54" s="5" t="s">
         <v>769</v>
       </c>
-      <c r="B54" s="2">
-        <v>0.5</v>
+      <c r="B54" s="6">
+        <v>0</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>846</v>
@@ -12358,12 +12305,14 @@
       <c r="Q54" s="2" t="s">
         <v>775</v>
       </c>
-      <c r="R54" s="6" t="s">
-        <v>854</v>
-      </c>
-      <c r="S54" s="2"/>
+      <c r="R54" s="8" t="s">
+        <v>861</v>
+      </c>
+      <c r="S54" s="6" t="s">
+        <v>851</v>
+      </c>
     </row>
-    <row r="55" spans="1:19" ht="409.6">
+    <row r="55" spans="1:19" ht="409.5">
       <c r="A55" s="3" t="s">
         <v>442</v>
       </c>
@@ -12418,7 +12367,7 @@
       </c>
       <c r="S55" s="2"/>
     </row>
-    <row r="56" spans="1:19" ht="409.6">
+    <row r="56" spans="1:19" ht="409.5">
       <c r="A56" s="3" t="s">
         <v>183</v>
       </c>
@@ -12473,7 +12422,7 @@
       </c>
       <c r="S56" s="2"/>
     </row>
-    <row r="57" spans="1:19" ht="409.6">
+    <row r="57" spans="1:19" ht="409.5">
       <c r="A57" s="3" t="s">
         <v>757</v>
       </c>
@@ -12528,7 +12477,7 @@
       </c>
       <c r="S57" s="2"/>
     </row>
-    <row r="58" spans="1:19" ht="409.6">
+    <row r="58" spans="1:19" ht="409.5">
       <c r="A58" s="3" t="s">
         <v>323</v>
       </c>
@@ -12539,7 +12488,7 @@
         <v>320</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>321</v>
@@ -12583,7 +12532,7 @@
       </c>
       <c r="S58" s="2"/>
     </row>
-    <row r="59" spans="1:19" ht="409.6">
+    <row r="59" spans="1:19" ht="409.5">
       <c r="A59" s="3" t="s">
         <v>684</v>
       </c>
@@ -12638,7 +12587,7 @@
       </c>
       <c r="S59" s="2"/>
     </row>
-    <row r="60" spans="1:19" ht="409.6">
+    <row r="60" spans="1:19" ht="409.5">
       <c r="A60" s="3" t="s">
         <v>505</v>
       </c>
@@ -12693,7 +12642,7 @@
       </c>
       <c r="S60" s="2"/>
     </row>
-    <row r="61" spans="1:19" ht="409.6">
+    <row r="61" spans="1:19" ht="409.5">
       <c r="A61" s="3" t="s">
         <v>252</v>
       </c>
@@ -12748,7 +12697,7 @@
       </c>
       <c r="S61" s="2"/>
     </row>
-    <row r="62" spans="1:19" ht="409.6">
+    <row r="62" spans="1:19" ht="409.5">
       <c r="A62" s="3" t="s">
         <v>820</v>
       </c>
@@ -12803,7 +12752,7 @@
       </c>
       <c r="S62" s="2"/>
     </row>
-    <row r="63" spans="1:19" ht="409.6">
+    <row r="63" spans="1:19" ht="409.5">
       <c r="A63" s="3" t="s">
         <v>337</v>
       </c>
@@ -12858,7 +12807,7 @@
       </c>
       <c r="S63" s="2"/>
     </row>
-    <row r="64" spans="1:19" ht="409.6">
+    <row r="64" spans="1:19" ht="409.5">
       <c r="A64" s="3" t="s">
         <v>696</v>
       </c>
@@ -12913,7 +12862,7 @@
       </c>
       <c r="S64" s="2"/>
     </row>
-    <row r="65" spans="1:19" ht="409.6">
+    <row r="65" spans="1:19" ht="409.5">
       <c r="A65" s="3" t="s">
         <v>516</v>
       </c>
@@ -12968,7 +12917,7 @@
       </c>
       <c r="S65" s="2"/>
     </row>
-    <row r="66" spans="1:19" ht="326" customHeight="1">
+    <row r="66" spans="1:19" ht="326.05" customHeight="1">
       <c r="A66" s="3" t="s">
         <v>22</v>
       </c>
@@ -13023,7 +12972,7 @@
       </c>
       <c r="S66" s="2"/>
     </row>
-    <row r="67" spans="1:19" ht="409.6">
+    <row r="67" spans="1:19" ht="409.5">
       <c r="A67" s="5" t="s">
         <v>596</v>
       </c>
@@ -13078,12 +13027,12 @@
       </c>
       <c r="S67" s="2"/>
     </row>
-    <row r="68" spans="1:19" ht="409.6">
+    <row r="68" spans="1:19" ht="409.5">
       <c r="A68" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B68" s="2">
-        <v>0.5</v>
+      <c r="B68" s="6">
+        <v>0</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>114</v>
@@ -13128,10 +13077,12 @@
       <c r="Q68" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="R68" s="6" t="s">
-        <v>852</v>
-      </c>
-      <c r="S68" s="7"/>
+      <c r="R68" s="8" t="s">
+        <v>860</v>
+      </c>
+      <c r="S68" s="6" t="s">
+        <v>851</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:S68" xr:uid="{1CCA9407-2158-4443-B762-15EB8023C913}"/>

</xml_diff>